<commit_message>
pbase pcb finalizado v1
</commit_message>
<xml_diff>
--- a/pcbs/pbase/PCB Layout Checklist_PBASE.xlsx
+++ b/pcbs/pbase/PCB Layout Checklist_PBASE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="93">
   <si>
     <t xml:space="preserve">Ubicación de componentes</t>
   </si>
@@ -118,9 +118,6 @@
     <t xml:space="preserve">1. Comunes digitales y analógicos unidos en un solo punto.</t>
   </si>
   <si>
-    <t xml:space="preserve">Tengo de ambos?</t>
-  </si>
-  <si>
     <t xml:space="preserve">2. Verificar pistas debajo de componentes ruidosos o sensibles.</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
     <t xml:space="preserve">8. Tolerancia de drills especificada.</t>
   </si>
   <si>
+    <t xml:space="preserve">Por defecto.</t>
+  </si>
+  <si>
     <t xml:space="preserve">9. Tolerancia de máscara antisoldante especificada.</t>
   </si>
   <si>
@@ -262,6 +262,9 @@
     <t xml:space="preserve">7. Verificar profundidad de la máscara antisoldante.</t>
   </si>
   <si>
+    <t xml:space="preserve">SE TRATA CON EL FABRICANTE</t>
+  </si>
+  <si>
     <t xml:space="preserve">8. Verificar el netlist manualmente o por inspección visual.</t>
   </si>
   <si>
@@ -271,9 +274,15 @@
     <t xml:space="preserve">10. Verificar si el origen de orificios es un pad de referencia.</t>
   </si>
   <si>
+    <t xml:space="preserve">PARA HACER A LO ÚLTIMO.</t>
+  </si>
+  <si>
     <t xml:space="preserve">11. Anotar en layer auxiliar ancho del PCB, material y peso del cobre.</t>
   </si>
   <si>
+    <t xml:space="preserve">FALTA ESTO</t>
+  </si>
+  <si>
     <t xml:space="preserve">12. Utilizar aislamiento térmico (thermal relief) en capas internas de distribución de alimentación.</t>
   </si>
   <si>
@@ -284,6 +293,9 @@
   </si>
   <si>
     <t xml:space="preserve">15. Definir correctamente el panelizado del PCB.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HACE FALTA?</t>
   </si>
   <si>
     <t xml:space="preserve">16. Encapsulados metálicos de cristales de alta frecuencia deberían conectarse a GND.</t>
@@ -361,7 +373,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +384,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -416,7 +434,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,6 +471,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -469,7 +495,7 @@
       <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -532,8 +558,8 @@
   </sheetPr>
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -738,18 +764,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="3"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
@@ -758,7 +784,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
@@ -767,7 +793,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
@@ -776,7 +802,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
@@ -785,7 +811,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
@@ -794,30 +820,34 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>1</v>
@@ -828,94 +858,128 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="B39" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="B41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="C42" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
@@ -928,110 +992,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="4"/>
+      <c r="C49" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="4"/>
+      <c r="C50" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="4"/>
+      <c r="C51" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-    </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="4"/>
+      <c r="C52" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="4"/>
+      <c r="C53" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="4"/>
+      <c r="C54" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
+      <c r="C56" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
+      <c r="C57" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
+      <c r="C58" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
+      <c r="C59" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -1044,117 +1138,149 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-    </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C61" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-    </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="3"/>
+      <c r="B67" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="C67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
+      <c r="C69" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B70" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="C70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="C71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-    </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B75" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="C75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
+      <c r="C76" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
PCB correcion pista 3V3
</commit_message>
<xml_diff>
--- a/pcbs/pbase/PCB Layout Checklist_PBASE.xlsx
+++ b/pcbs/pbase/PCB Layout Checklist_PBASE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="98">
   <si>
     <t xml:space="preserve">Ubicación de componentes</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">1. Orientación consistente de componentes SMD</t>
   </si>
   <si>
+    <t xml:space="preserve">Todos los resistores SMD verticales. SD horizontal.</t>
+  </si>
+  <si>
     <t xml:space="preserve">.Cumple</t>
   </si>
   <si>
@@ -64,12 +67,15 @@
     <t xml:space="preserve">7. Capacitores de desacople (bypass) cerca de pines de alimentación de los IC</t>
   </si>
   <si>
+    <t xml:space="preserve">No hay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.No Aplica</t>
+  </si>
+  <si>
     <t xml:space="preserve">8. Verificar terminadores en serie cercanos a la fuente</t>
   </si>
   <si>
-    <t xml:space="preserve">.No Aplica</t>
-  </si>
-  <si>
     <t xml:space="preserve">9. Drivers I/O cercanos a donde las señales abandonan el PCB</t>
   </si>
   <si>
@@ -100,13 +106,13 @@
     <t xml:space="preserve">16. Verificar factor de forma de los pads SMD.</t>
   </si>
   <si>
-    <t xml:space="preserve">SD MISMO QUE EN INFOTRONIC SD </t>
+    <t xml:space="preserve">SD MISMO QUE EN INFOTRONIC  </t>
   </si>
   <si>
     <t xml:space="preserve">17. Fiduciales para ensamle automático.</t>
   </si>
   <si>
-    <t xml:space="preserve">PODRIA NO TENERLOS! ES PARA ENSAMBLE AUTOMATICO</t>
+    <t xml:space="preserve">Podría no tenerlos! Es para ensamble automático. Lo ensamblaremos a mano.</t>
   </si>
   <si>
     <t xml:space="preserve">18. Distancia de seguridad suficiente para ICs con zócalo.</t>
@@ -118,6 +124,9 @@
     <t xml:space="preserve">1. Comunes digitales y analógicos unidos en un solo punto.</t>
   </si>
   <si>
+    <t xml:space="preserve">Solo tengo un común.</t>
+  </si>
+  <si>
     <t xml:space="preserve">2. Verificar pistas debajo de componentes ruidosos o sensibles.</t>
   </si>
   <si>
@@ -127,6 +136,9 @@
     <t xml:space="preserve">4. Verificar pistas susceptibles a puentes de soldadura.</t>
   </si>
   <si>
+    <t xml:space="preserve">Distancia entre pista y LPC?</t>
+  </si>
+  <si>
     <t xml:space="preserve">5. Verificar pistas sin conexión en un extremo, a menos que sea a propósito.</t>
   </si>
   <si>
@@ -145,6 +157,9 @@
     <t xml:space="preserve">9. Utilizar planos de GND donde sea posible.</t>
   </si>
   <si>
+    <t xml:space="preserve">TOP y BOTTOM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dimensiones</t>
   </si>
   <si>
@@ -280,7 +295,7 @@
     <t xml:space="preserve">11. Anotar en layer auxiliar ancho del PCB, material y peso del cobre.</t>
   </si>
   <si>
-    <t xml:space="preserve">FALTA ESTO</t>
+    <t xml:space="preserve">ANCHO PCB, MATERIAL, PESO. (MATERIAL: FR4)</t>
   </si>
   <si>
     <t xml:space="preserve">12. Utilizar aislamiento térmico (thermal relief) en capas internas de distribución de alimentación.</t>
@@ -434,7 +449,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -465,10 +480,6 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -558,8 +569,8 @@
   </sheetPr>
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -585,177 +596,181 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1</v>
@@ -766,88 +781,92 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C21" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C29" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>1</v>
@@ -858,132 +877,132 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>1</v>
@@ -994,142 +1013,142 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>1</v>
@@ -1140,146 +1159,146 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="C70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>91</v>
+        <v>95</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="C75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>